<commit_message>
added css and javascript
</commit_message>
<xml_diff>
--- a/cv_information.xlsx
+++ b/cv_information.xlsx
@@ -432,6 +432,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="100" customWidth="1" min="1" max="1"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -443,7 +446,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>AKASH GOELMobile: 9310631244, E-Mail: akashg2494@gmail.com7 years of experience in banking across various fields like credit analysis, credit approvals, credit underwriting and appraisals. My eagerness to learn has helped me explore different job profiles which in turn have broadened my point of view.  	WORK EXPERIENCE	IDFC First Bank- Manager (Underwriting- Education Loan), Rajendra PlaceSeptember 2022- PresentRecommendation after Assessing the creditworthiness of customers, minimizing debt losses, increasing sales, investigating credit applications to better understand how much risk could be involved in extending credit to the customer.Ensuring the best tat with a hassle-free process and minimal paperwork.Making the real-time decision cases to make sure all the decisions as per the current credit Policy.Monitoring Delinquency for PAN India every month.Publishing MIS for the Bounce data on monthly basis.Making the details Root Cause Analysis for the bounce cases and sharing the feedback with PAN India credit team, how we could have appraised case at the time of underwriting.Axis Bank – Deputy Manager (Underwriting – Credit Cards), NoidaAugust 2021- September 2022Executing credit underwriting activities and overcoming complex business challenges using experience-backed judgment, strong work ethics and irreproachable integrity.Processing all card proposals and sanction as per bank norms with help of evaluating factors (CIBIL, ITR, Past Track) other variable factors and bank product.Check risk level for individual applicant. HDFC Bank – Deputy Manager (Underwriting – Credit Cards, Auto Loan), DelhiSep 2019 – August 2021Credit underwriting in view of financial health of the Individuals after scrutinizing financial and other policy parameters.Processing all proposals and sanction as per bank norms with help of evaluating factors (CIBIL, ITR, PAST Track) other variable factors and bank product.Review detailed historical and projected financial analysis utilizing tax returns, financial statements, and other income documents.Taking logical and sensible calls on deviations and minimize errors.Coordinating with major stakeholders like Sales team, Branch, DIP, Quality and Policy teams.Portfolio Analysis of the channel wise delinquency and product wise delinquency.Underwriting – Restructuring loan (AL, PL and CC)Examine the entire credit application and check all information whether all criteria fulfill or not as per policy.Calling to applicant and understanding the situation, reason for applying restructuring loan.Adhering RBI guidelines for the restructuring.Review and analyze special conditions, Credit card deficiencies and exception requests to determine appropriate courses of action.WNS Global Services – Senior Associate (Underwriting - Education loan), Gurugram, January 2018 – Aug 2019Evaluated financial strength of individuals and businesses by analyzing credit bureau report &amp; financial statementsResponsible for the timely review and disposition of conforming education loan applications.Worked within company guidelines to make calculations for qualifying and administered decisions using proprietary loan origination systems.Ensured compliance amidst continuously changing underwriting scenarios for an international process.Improved process efficiency by developing spreadsheets that managed all aspects of the loan review and limited data validation errors.Effectively managed pipeline of over 25 schools to meet strict deadlines while personally guiding clients through the underwriting process.Xceedance Consulting India Private Limited - Analyst (Underwriting), Gurugram, India                                      June 2016 to Dec 2017Providing Underwriting support to the underwriters (Berkshire Hathaway Specialty Insurance Company and Hallmark Insurance Group).Creating submissions and Quotes (Property and Aviation Lines of Business) for Hallmark Insurance Group.Conducting Audits/Quality Checks of the Submissions processed by the team members.Achieving Quality Standards &amp; SLA as committed to clients.Monitor work and manage daily work volumes and leverage cross trainings.Prepare standard operating procedures (SOP) and work flow of the process.Providing training to the new joiners in the team. 	ACHIEVEMENTS	Won June 2023 best Credit Manager Award in IDFC Bank.Won Best credit Manager in Axis bank.Achieved less than 1% error rate in HDFC and Axis.Won Silver Star in HDFC Bank.Selected for pilot project within 6months working with Xceedance.	KEY STRENGTHS AND SKILLS	Ability to inspire and guide team.Quick learner and analytical Decision maker.Efficient organizational skills with the ability to prioritize multiple concurrent demands.Positive Time Management and People Management Skills.Highly motivated self-starter. 	ACADEMIC CREDENTIALS	Master of Business Administration in Finance and Marketing from Delhi Institute of Advanced Studies of IP University, 2014-2016.Bachelor of Business Administration from Ideal Institute of Management and Technology of IP University, 2011-2014.XII from Rishabh Public School, Mayur Vihar, New Delhi, CBSE Board in  2011.X from Rishabh Public School, Mayur Vihar, New Delhi, CBSE Board in  2009.</t>
+          <t>. Aarushi Rohatgi 999-921-8543 aarushi.9999218543@gmail.com Credit Analyst and outstanding performer in collections, sales and customer service within banking and BPO industry. Proven success in leadership, operational excellence and organizational development with keen understanding of elements of banking. Recognized for inspiring management team members to excel and encouraging creative work environments. Excellent communication skills and great understanding of customers need and requirement. Skills MS Office Suite Intermediate Risk management Advanced Team leadership Intermediate Customer relations Advanced Collections processing Advanced Financial product knowledge Upper intermediate Revenue generations Upper intermediate Relationship building and management Upper intermediate Business develoment Intermediate Time management Advanced Work History 2018-11 - 2023-04 AMERICAN EXPRESS, Gurugram • Handling 120-200 inbound calls daily with a goal of serving the best solution to customer's need with collecting the owed debt if required .. • Handled 400-500 outbound calls daily with goal of collecting owed debt. • Researched accounts and completed due diligence to resolve collection problems. • Achieved performance goals on consistent basis. Counseled debtors on payment options and arranged installment agreements. • Processed payments and contracts on accounts. Trained new team members on performance strategies and provided mentoring. • Discussed options with delinquent clients in terms of proposed solutions or foreclosure. • Negotiated to collect balance in full. Processed payments and applied to customer balances. • Used probing techniques to determine debtors' reasons for delinquency. • Recorded all information regarding financial status of customers. • Devoted special emphasis to punctuality and worked to maintain outstanding attendance record, consistently arriving to work ready to start immediately. • Developed team communications and information for team meetings 2017-08 - 2018-10 RESERVATION ASSOCIATE LEELA RESERVATIONS WORLD WIDE , GURUGRAM • Managed and closed reservation calls to increase bookings by maintaining strong knowledge of resort products, services and facilities. • Arranged for group hotel bookings in collaboration with sales department for weddings and special events. • Provided high level of customer service to each person by engaging customer and using active listening and effective interpersonal skills. • Informed clients of essential travel information, such as travel times, transportation connections, medical and visa requirements to facilitate quality service. • Answered incoming phone calls and developed friendly rapport with callers while answering questions, making recommendations and leading conversations to bookings. • Managed online booking inquiries and assisted guests and travel partners with questions throughout entire booking cycle. • Managed quality assurance program including on site evaluations, internal audits and customer surveys. .. Education 2000-01 - 2014-06 High School Diploma DPS MATHURA ROAD SCHOOL - New Delhi Higher Senior Secondary (Class XII); Affiliated to CBSE Board 2014 2014-06 - 2018-06 B.Com Indra Gandhi University - New Delhi • Graduated with 65% GPA 2020-06 - 2022-06 MBA: Marketing Narsee Monjee College of Commerce And Economics - Mumbai • Professional development completed in Marketing. Languages English &amp; Hindi .</t>
         </is>
       </c>
     </row>

</xml_diff>